<commit_message>
last commit web's first stage
</commit_message>
<xml_diff>
--- a/project/白维扬/测试用例1.xlsx
+++ b/project/白维扬/测试用例1.xlsx
@@ -547,9 +547,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -588,25 +588,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -618,9 +604,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -634,9 +619,85 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -651,67 +712,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -757,174 +757,174 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -950,15 +950,6 @@
         <color theme="1"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1004,17 +995,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1026,21 +1017,6 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1059,157 +1035,172 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1238,9 +1229,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1562,10 +1550,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:C243"/>
+  <dimension ref="A1:C189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="C142" sqref="C142"/>
+    <sheetView tabSelected="1" topLeftCell="A170" workbookViewId="0">
+      <selection activeCell="C192" sqref="C192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelCol="2"/>
@@ -3086,330 +3074,6 @@
         <v>174</v>
       </c>
     </row>
-    <row r="190" spans="2:3">
-      <c r="B190" s="6">
-        <v>185</v>
-      </c>
-      <c r="C190" s="6"/>
-    </row>
-    <row r="191" spans="2:3">
-      <c r="B191" s="7">
-        <v>186</v>
-      </c>
-      <c r="C191" s="7"/>
-    </row>
-    <row r="192" spans="2:3">
-      <c r="B192" s="6">
-        <v>187</v>
-      </c>
-      <c r="C192" s="6"/>
-    </row>
-    <row r="193" spans="2:3">
-      <c r="B193" s="7">
-        <v>188</v>
-      </c>
-      <c r="C193" s="7"/>
-    </row>
-    <row r="194" spans="2:3">
-      <c r="B194" s="6">
-        <v>189</v>
-      </c>
-      <c r="C194" s="6"/>
-    </row>
-    <row r="195" spans="2:3">
-      <c r="B195" s="7">
-        <v>190</v>
-      </c>
-      <c r="C195" s="7"/>
-    </row>
-    <row r="196" spans="2:3">
-      <c r="B196" s="6">
-        <v>191</v>
-      </c>
-      <c r="C196" s="6"/>
-    </row>
-    <row r="197" spans="2:3">
-      <c r="B197" s="7">
-        <v>192</v>
-      </c>
-      <c r="C197" s="7"/>
-    </row>
-    <row r="198" spans="2:3">
-      <c r="B198" s="6">
-        <v>193</v>
-      </c>
-      <c r="C198" s="6"/>
-    </row>
-    <row r="199" spans="2:3">
-      <c r="B199" s="7">
-        <v>194</v>
-      </c>
-      <c r="C199" s="7"/>
-    </row>
-    <row r="200" spans="2:3">
-      <c r="B200" s="6">
-        <v>195</v>
-      </c>
-      <c r="C200" s="6"/>
-    </row>
-    <row r="201" spans="2:3">
-      <c r="B201" s="7">
-        <v>196</v>
-      </c>
-      <c r="C201" s="7"/>
-    </row>
-    <row r="202" spans="2:3">
-      <c r="B202" s="6">
-        <v>197</v>
-      </c>
-      <c r="C202" s="6"/>
-    </row>
-    <row r="203" spans="2:3">
-      <c r="B203" s="7">
-        <v>198</v>
-      </c>
-      <c r="C203" s="7"/>
-    </row>
-    <row r="204" spans="2:3">
-      <c r="B204" s="6">
-        <v>199</v>
-      </c>
-      <c r="C204" s="6"/>
-    </row>
-    <row r="205" spans="2:3">
-      <c r="B205" s="7">
-        <v>200</v>
-      </c>
-      <c r="C205" s="7"/>
-    </row>
-    <row r="206" spans="2:3">
-      <c r="B206" s="6">
-        <v>201</v>
-      </c>
-      <c r="C206" s="6"/>
-    </row>
-    <row r="207" spans="2:3">
-      <c r="B207" s="7">
-        <v>202</v>
-      </c>
-      <c r="C207" s="7"/>
-    </row>
-    <row r="208" spans="2:3">
-      <c r="B208" s="6">
-        <v>203</v>
-      </c>
-      <c r="C208" s="6"/>
-    </row>
-    <row r="209" spans="2:3">
-      <c r="B209" s="7">
-        <v>204</v>
-      </c>
-      <c r="C209" s="7"/>
-    </row>
-    <row r="210" spans="2:3">
-      <c r="B210" s="6">
-        <v>205</v>
-      </c>
-      <c r="C210" s="6"/>
-    </row>
-    <row r="211" spans="2:3">
-      <c r="B211" s="7">
-        <v>206</v>
-      </c>
-      <c r="C211" s="7"/>
-    </row>
-    <row r="212" spans="2:3">
-      <c r="B212" s="6">
-        <v>207</v>
-      </c>
-      <c r="C212" s="6"/>
-    </row>
-    <row r="213" spans="2:3">
-      <c r="B213" s="7">
-        <v>208</v>
-      </c>
-      <c r="C213" s="7"/>
-    </row>
-    <row r="214" spans="2:3">
-      <c r="B214" s="6">
-        <v>209</v>
-      </c>
-      <c r="C214" s="6"/>
-    </row>
-    <row r="215" spans="2:3">
-      <c r="B215" s="7">
-        <v>210</v>
-      </c>
-      <c r="C215" s="7"/>
-    </row>
-    <row r="216" spans="2:3">
-      <c r="B216" s="6">
-        <v>211</v>
-      </c>
-      <c r="C216" s="6"/>
-    </row>
-    <row r="217" spans="2:3">
-      <c r="B217" s="7">
-        <v>212</v>
-      </c>
-      <c r="C217" s="7"/>
-    </row>
-    <row r="218" spans="2:3">
-      <c r="B218" s="6">
-        <v>213</v>
-      </c>
-      <c r="C218" s="6"/>
-    </row>
-    <row r="219" spans="2:3">
-      <c r="B219" s="7">
-        <v>214</v>
-      </c>
-      <c r="C219" s="7"/>
-    </row>
-    <row r="220" spans="2:3">
-      <c r="B220" s="6">
-        <v>215</v>
-      </c>
-      <c r="C220" s="6"/>
-    </row>
-    <row r="221" spans="2:3">
-      <c r="B221" s="7">
-        <v>216</v>
-      </c>
-      <c r="C221" s="7"/>
-    </row>
-    <row r="222" spans="2:3">
-      <c r="B222" s="6">
-        <v>217</v>
-      </c>
-      <c r="C222" s="6"/>
-    </row>
-    <row r="223" spans="2:3">
-      <c r="B223" s="7">
-        <v>218</v>
-      </c>
-      <c r="C223" s="7"/>
-    </row>
-    <row r="224" spans="2:3">
-      <c r="B224" s="6">
-        <v>219</v>
-      </c>
-      <c r="C224" s="6"/>
-    </row>
-    <row r="225" spans="2:3">
-      <c r="B225" s="7">
-        <v>220</v>
-      </c>
-      <c r="C225" s="7"/>
-    </row>
-    <row r="226" spans="2:3">
-      <c r="B226" s="6">
-        <v>221</v>
-      </c>
-      <c r="C226" s="6"/>
-    </row>
-    <row r="227" spans="2:3">
-      <c r="B227" s="7">
-        <v>222</v>
-      </c>
-      <c r="C227" s="7"/>
-    </row>
-    <row r="228" spans="2:3">
-      <c r="B228" s="6">
-        <v>223</v>
-      </c>
-      <c r="C228" s="6"/>
-    </row>
-    <row r="229" spans="2:3">
-      <c r="B229" s="7">
-        <v>224</v>
-      </c>
-      <c r="C229" s="7"/>
-    </row>
-    <row r="230" spans="2:3">
-      <c r="B230" s="6">
-        <v>225</v>
-      </c>
-      <c r="C230" s="6"/>
-    </row>
-    <row r="231" spans="2:3">
-      <c r="B231" s="7">
-        <v>226</v>
-      </c>
-      <c r="C231" s="7"/>
-    </row>
-    <row r="232" spans="2:3">
-      <c r="B232" s="6">
-        <v>227</v>
-      </c>
-      <c r="C232" s="6"/>
-    </row>
-    <row r="233" spans="2:3">
-      <c r="B233" s="10">
-        <v>228</v>
-      </c>
-      <c r="C233" s="10"/>
-    </row>
-    <row r="234" spans="2:3">
-      <c r="B234" s="6">
-        <v>229</v>
-      </c>
-      <c r="C234" s="6"/>
-    </row>
-    <row r="235" spans="2:3">
-      <c r="B235" s="7">
-        <v>230</v>
-      </c>
-      <c r="C235" s="7"/>
-    </row>
-    <row r="236" spans="2:3">
-      <c r="B236" s="6">
-        <v>231</v>
-      </c>
-      <c r="C236" s="6"/>
-    </row>
-    <row r="237" spans="2:3">
-      <c r="B237" s="7">
-        <v>232</v>
-      </c>
-      <c r="C237" s="7"/>
-    </row>
-    <row r="238" spans="2:3">
-      <c r="B238" s="6">
-        <v>233</v>
-      </c>
-      <c r="C238" s="6"/>
-    </row>
-    <row r="239" spans="2:3">
-      <c r="B239" s="7">
-        <v>234</v>
-      </c>
-      <c r="C239" s="7"/>
-    </row>
-    <row r="240" spans="2:3">
-      <c r="B240" s="6">
-        <v>235</v>
-      </c>
-      <c r="C240" s="6"/>
-    </row>
-    <row r="241" spans="2:3">
-      <c r="B241" s="7">
-        <v>236</v>
-      </c>
-      <c r="C241" s="7"/>
-    </row>
-    <row r="242" spans="2:3">
-      <c r="B242" s="6">
-        <v>237</v>
-      </c>
-      <c r="C242" s="6"/>
-    </row>
-    <row r="243" spans="2:3">
-      <c r="B243" s="7">
-        <v>238</v>
-      </c>
-      <c r="C243" s="10"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>